<commit_message>
Added bar codes for Irminger D3
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GI02HYPM_00003.xlsx
+++ b/deployment/Omaha_Cal_Info_GI02HYPM_00003.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="520" windowWidth="23040" windowHeight="12120"/>
+    <workbookView xWindow="555" yWindow="525" windowWidth="23040" windowHeight="12120"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -17,7 +22,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="81">
   <si>
     <t>Ref Des</t>
   </si>
@@ -240,6 +245,36 @@
   </si>
   <si>
     <t>CC_ctcor</t>
+  </si>
+  <si>
+    <t>OL000597</t>
+  </si>
+  <si>
+    <t>N00115</t>
+  </si>
+  <si>
+    <t>N00114</t>
+  </si>
+  <si>
+    <t>N00113</t>
+  </si>
+  <si>
+    <t>N00116</t>
+  </si>
+  <si>
+    <t>OL000598</t>
+  </si>
+  <si>
+    <t>OL000599</t>
+  </si>
+  <si>
+    <t>A01398</t>
+  </si>
+  <si>
+    <t>A00630</t>
+  </si>
+  <si>
+    <t>OL000600</t>
   </si>
 </sst>
 </file>
@@ -247,11 +282,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="34" x14ac:knownFonts="1">
     <font>
@@ -470,6 +505,7 @@
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -632,14 +668,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -740,7 +776,7 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -778,7 +814,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -796,7 +832,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -820,7 +856,7 @@
     <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
@@ -864,7 +900,7 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="57" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="15" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -907,9 +943,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -947,13 +980,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="33" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -962,7 +995,7 @@
     <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1151,7 +1184,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Read Me"/>
@@ -1457,29 +1490,29 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="8" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="19" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="13.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.6640625" style="8" customWidth="1"/>
-    <col min="13" max="13" width="17.1640625" style="8" customWidth="1"/>
-    <col min="14" max="14" width="17.83203125" style="8" customWidth="1"/>
-    <col min="15" max="16384" width="8.83203125" style="8"/>
+    <col min="2" max="2" width="16.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="19" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="8" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" style="8" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" style="8" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" style="8" customWidth="1"/>
+    <col min="15" max="16384" width="8.85546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="28">
+    <row r="1" spans="1:14" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
         <v>38</v>
       </c>
@@ -1519,109 +1552,111 @@
       <c r="M1" s="35"/>
       <c r="N1" s="35"/>
     </row>
-    <row r="2" spans="1:14" s="20" customFormat="1">
-      <c r="A2" s="73"/>
-      <c r="B2" s="70" t="s">
+    <row r="2" spans="1:14" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="70" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="70">
-        <v>3</v>
-      </c>
-      <c r="E2" s="74">
+      <c r="C2" s="69" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="69">
+        <v>3</v>
+      </c>
+      <c r="E2" s="73">
         <v>42562</v>
       </c>
-      <c r="F2" s="75">
+      <c r="F2" s="74">
         <v>0.59861111111111109</v>
       </c>
-      <c r="G2" s="76">
+      <c r="G2" s="75">
         <v>42948</v>
       </c>
-      <c r="H2" s="70">
+      <c r="H2" s="69">
         <v>59.969499999999996</v>
       </c>
-      <c r="I2" s="70">
+      <c r="I2" s="69">
         <v>-39.488599999999998</v>
       </c>
-      <c r="J2" s="70">
+      <c r="J2" s="69">
         <v>2673</v>
       </c>
-      <c r="K2" s="70" t="s">
+      <c r="K2" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="71"/>
+      <c r="L2" s="70"/>
       <c r="M2" s="36"/>
       <c r="N2" s="36"/>
     </row>
-    <row r="3" spans="1:14" s="20" customFormat="1">
-      <c r="A3" s="77"/>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
-    </row>
-    <row r="4" spans="1:14" customFormat="1">
-      <c r="A4" s="73"/>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-    </row>
-    <row r="5" spans="1:14" customFormat="1"/>
-    <row r="6" spans="1:14" customFormat="1"/>
-    <row r="7" spans="1:14" customFormat="1"/>
-    <row r="8" spans="1:14" customFormat="1"/>
-    <row r="9" spans="1:14" customFormat="1"/>
-    <row r="10" spans="1:14" customFormat="1"/>
-    <row r="11" spans="1:14" s="20" customFormat="1">
+    <row r="3" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="76"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="76"/>
+    </row>
+    <row r="4" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="72"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="72"/>
+      <c r="M4" s="72"/>
+    </row>
+    <row r="5" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E11" s="26"/>
       <c r="F11" s="27"/>
       <c r="G11" s="26"/>
     </row>
-    <row r="12" spans="1:14" s="20" customFormat="1">
+    <row r="12" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E12" s="26"/>
       <c r="F12" s="27"/>
       <c r="G12" s="26"/>
     </row>
-    <row r="13" spans="1:14" s="20" customFormat="1">
+    <row r="13" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E13" s="26"/>
       <c r="F13" s="27"/>
       <c r="G13" s="26"/>
     </row>
-    <row r="14" spans="1:14" s="20" customFormat="1">
+    <row r="14" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E14" s="26"/>
       <c r="F14" s="27"/>
       <c r="G14" s="26"/>
     </row>
-    <row r="15" spans="1:14" s="20" customFormat="1">
+    <row r="15" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E15" s="26"/>
       <c r="F15" s="27"/>
       <c r="G15" s="26"/>
     </row>
-    <row r="16" spans="1:14" s="20" customFormat="1">
+    <row r="16" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E16" s="26"/>
       <c r="F16" s="27"/>
       <c r="G16" s="26"/>
     </row>
-    <row r="17" spans="5:7" s="20" customFormat="1">
+    <row r="17" spans="5:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E17" s="26"/>
       <c r="F17" s="27"/>
       <c r="G17" s="26"/>
@@ -1643,26 +1678,26 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H25" sqref="H25:H26"/>
+      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="18" customWidth="1"/>
     <col min="5" max="5" width="11" style="12" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="29.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.5" style="3" customWidth="1"/>
-    <col min="9" max="9" width="41.6640625" style="12" customWidth="1"/>
-    <col min="10" max="13" width="10.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="41.7109375" style="12" customWidth="1"/>
+    <col min="10" max="13" width="10.7109375" style="3" customWidth="1"/>
     <col min="14" max="14" width="5" style="3" customWidth="1"/>
-    <col min="15" max="16384" width="8.83203125" style="3"/>
+    <col min="15" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="17" customFormat="1" ht="28">
+    <row r="1" spans="1:9" s="17" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1691,7 +1726,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="17" customFormat="1">
+    <row r="2" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="47"/>
@@ -1702,112 +1737,132 @@
       <c r="H2" s="16"/>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B3"/>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
       <c r="C3" s="48" t="s">
         <v>44</v>
       </c>
       <c r="D3" s="18">
         <v>3</v>
       </c>
-      <c r="E3"/>
-      <c r="F3" s="65">
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="64">
         <v>3280</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="67">
+      <c r="H3" s="66">
         <v>45</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B4"/>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
       <c r="C4" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D4" s="51">
         <v>3</v>
       </c>
-      <c r="E4"/>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
       <c r="F4" s="54">
         <v>3280</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="68">
+      <c r="H4" s="67">
         <v>1.533E-6</v>
       </c>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B5"/>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
       <c r="C5" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D5" s="51">
         <v>3</v>
       </c>
-      <c r="E5"/>
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
       <c r="F5" s="54">
         <v>3280</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="67">
+      <c r="H5" s="66">
         <v>46</v>
       </c>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B6"/>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
       <c r="C6" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="51">
         <v>3</v>
       </c>
-      <c r="E6"/>
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
       <c r="F6" s="54">
         <v>3280</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="68">
+      <c r="H6" s="67">
         <v>6.7999999999999996E-3</v>
       </c>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B7"/>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
       <c r="C7" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D7" s="51">
         <v>3</v>
       </c>
-      <c r="E7"/>
+      <c r="E7" t="s">
+        <v>72</v>
+      </c>
       <c r="F7" s="54">
         <v>3280</v>
       </c>
@@ -1821,18 +1876,22 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B8"/>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
       <c r="C8" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D8" s="51">
         <v>3</v>
       </c>
-      <c r="E8"/>
+      <c r="E8" t="s">
+        <v>72</v>
+      </c>
       <c r="F8" s="54">
         <v>3280</v>
       </c>
@@ -1846,18 +1905,22 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B9"/>
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
       <c r="C9" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D9" s="51">
         <v>3</v>
       </c>
-      <c r="E9"/>
+      <c r="E9" t="s">
+        <v>72</v>
+      </c>
       <c r="F9" s="54">
         <v>3280</v>
       </c>
@@ -1871,18 +1934,22 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B10"/>
+      <c r="B10" t="s">
+        <v>71</v>
+      </c>
       <c r="C10" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D10" s="51">
         <v>3</v>
       </c>
-      <c r="E10"/>
+      <c r="E10" t="s">
+        <v>72</v>
+      </c>
       <c r="F10" s="54">
         <v>3280</v>
       </c>
@@ -1896,7 +1963,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="32"/>
       <c r="C11" s="49"/>
@@ -1907,166 +1974,190 @@
       <c r="H11" s="7"/>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B12"/>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
       <c r="C12" s="48" t="s">
         <v>44</v>
       </c>
       <c r="D12" s="18">
         <v>3</v>
       </c>
-      <c r="E12"/>
-      <c r="F12" s="65">
+      <c r="E12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="64">
         <v>1476</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="72">
+      <c r="H12" s="71">
         <v>59.969499999999996</v>
       </c>
       <c r="I12" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B13"/>
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
       <c r="C13" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D13" s="51">
         <v>3</v>
       </c>
-      <c r="E13"/>
+      <c r="E13" t="s">
+        <v>73</v>
+      </c>
       <c r="F13" s="54">
         <v>1476</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="72">
+      <c r="H13" s="71">
         <v>-39.488599999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="32"/>
       <c r="C14" s="49"/>
       <c r="D14" s="51"/>
       <c r="E14" s="4"/>
       <c r="F14" s="29"/>
-      <c r="G14" s="69"/>
+      <c r="G14" s="68"/>
       <c r="H14" s="45"/>
       <c r="I14" s="45"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B15"/>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
       <c r="C15" s="48" t="s">
         <v>44</v>
       </c>
       <c r="D15" s="18">
         <v>3</v>
       </c>
-      <c r="E15"/>
-      <c r="F15" s="65">
+      <c r="E15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="64">
         <v>131</v>
       </c>
-      <c r="G15" s="69" t="s">
+      <c r="G15" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="72">
+      <c r="H15" s="71">
         <v>59.969499999999996</v>
       </c>
-      <c r="I15" s="70"/>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="I15" s="69"/>
+    </row>
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B16"/>
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
       <c r="C16" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D16" s="51">
         <v>3</v>
       </c>
-      <c r="E16"/>
+      <c r="E16" t="s">
+        <v>74</v>
+      </c>
       <c r="F16" s="54">
         <v>131</v>
       </c>
-      <c r="G16" s="69" t="s">
+      <c r="G16" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="72">
+      <c r="H16" s="71">
         <v>-39.488599999999998</v>
       </c>
       <c r="I16" s="45"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="32"/>
       <c r="C17" s="49"/>
       <c r="D17" s="51"/>
       <c r="E17" s="4"/>
       <c r="F17" s="29"/>
-      <c r="G17" s="69"/>
+      <c r="G17" s="68"/>
       <c r="H17" s="45"/>
       <c r="I17" s="45"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B18"/>
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
       <c r="C18" s="48" t="s">
         <v>44</v>
       </c>
       <c r="D18" s="18">
         <v>3</v>
       </c>
-      <c r="E18"/>
-      <c r="F18" s="65">
+      <c r="E18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="64">
         <v>1109</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="72">
+      <c r="H18" s="71">
         <v>59.969499999999996</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B19"/>
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
       <c r="C19" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D19" s="51">
         <v>3</v>
       </c>
-      <c r="E19"/>
+      <c r="E19" t="s">
+        <v>75</v>
+      </c>
       <c r="F19" s="54">
         <v>1109</v>
       </c>
       <c r="G19" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="72">
+      <c r="H19" s="71">
         <v>-39.488599999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="32"/>
       <c r="C20" s="49"/>
@@ -2076,16 +2167,21 @@
       <c r="G20" s="11"/>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B21"/>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
       <c r="C21" s="55" t="s">
         <v>44</v>
       </c>
       <c r="D21" s="18">
         <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>76</v>
       </c>
       <c r="F21" s="58">
         <v>55094</v>
@@ -2093,23 +2189,28 @@
       <c r="G21" s="11"/>
       <c r="H21" s="12"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B22" s="32"/>
       <c r="C22" s="55"/>
       <c r="F22" s="56"/>
       <c r="G22" s="11"/>
       <c r="H22" s="12"/>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B23"/>
+      <c r="B23" t="s">
+        <v>71</v>
+      </c>
       <c r="C23" s="55" t="s">
         <v>44</v>
       </c>
       <c r="D23" s="18">
         <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>77</v>
       </c>
       <c r="F23" s="58">
         <v>55095</v>
@@ -2117,634 +2218,715 @@
       <c r="G23" s="11"/>
       <c r="H23" s="12"/>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C24" s="57"/>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
       <c r="I24" s="30"/>
       <c r="J24" s="28"/>
-      <c r="K24" s="12"/>
       <c r="N24" s="12"/>
       <c r="O24" s="31"/>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B25"/>
+      <c r="B25" t="s">
+        <v>71</v>
+      </c>
       <c r="C25" s="48" t="s">
         <v>44</v>
       </c>
       <c r="D25" s="18">
         <v>3</v>
       </c>
-      <c r="E25"/>
+      <c r="E25" t="s">
+        <v>78</v>
+      </c>
       <c r="F25" s="53" t="s">
         <v>47</v>
       </c>
       <c r="G25" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="72">
+      <c r="H25" s="71">
         <v>59.969499999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B26"/>
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
       <c r="C26" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D26" s="51">
         <v>3</v>
       </c>
-      <c r="E26"/>
+      <c r="E26" t="s">
+        <v>78</v>
+      </c>
       <c r="F26" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H26" s="72">
+      <c r="H26" s="71">
         <v>-39.488599999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B27"/>
+      <c r="B27" t="s">
+        <v>71</v>
+      </c>
       <c r="C27" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D27" s="51">
         <v>3</v>
       </c>
-      <c r="E27"/>
+      <c r="E27" t="s">
+        <v>78</v>
+      </c>
       <c r="F27" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G27" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="H27" s="63">
+      <c r="H27" s="62">
         <v>1450</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B28"/>
+      <c r="B28" t="s">
+        <v>71</v>
+      </c>
       <c r="C28" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D28" s="51">
         <v>3</v>
       </c>
-      <c r="E28"/>
+      <c r="E28" t="s">
+        <v>78</v>
+      </c>
       <c r="F28" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H28" s="61">
+      <c r="H28" s="60">
         <v>-6.7825760000000004E-8</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B29"/>
+      <c r="B29" t="s">
+        <v>71</v>
+      </c>
       <c r="C29" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D29" s="51">
         <v>3</v>
       </c>
-      <c r="E29"/>
+      <c r="E29" t="s">
+        <v>78</v>
+      </c>
       <c r="F29" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="H29" s="62">
+      <c r="H29" s="61">
         <v>-8.6661830000000006E-5</v>
       </c>
       <c r="I29" s="59"/>
-      <c r="K29" s="60"/>
-    </row>
-    <row r="30" spans="1:15">
+    </row>
+    <row r="30" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B30"/>
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
       <c r="C30" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D30" s="51">
         <v>3</v>
       </c>
-      <c r="E30"/>
+      <c r="E30" t="s">
+        <v>78</v>
+      </c>
       <c r="F30" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="H30" s="62">
+      <c r="H30" s="61">
         <v>3.015715E-4</v>
       </c>
       <c r="I30" s="59"/>
-      <c r="K30" s="60"/>
-    </row>
-    <row r="31" spans="1:15">
+    </row>
+    <row r="31" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B31"/>
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
       <c r="C31" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D31" s="51">
         <v>3</v>
       </c>
-      <c r="E31"/>
+      <c r="E31" t="s">
+        <v>78</v>
+      </c>
       <c r="F31" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="H31" s="62">
+      <c r="H31" s="61">
         <v>-4.0324660000000003E-6</v>
       </c>
       <c r="I31" s="59"/>
-      <c r="K31" s="60"/>
-    </row>
-    <row r="32" spans="1:15">
+    </row>
+    <row r="32" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B32"/>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
       <c r="C32" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D32" s="51">
         <v>3</v>
       </c>
-      <c r="E32"/>
+      <c r="E32" t="s">
+        <v>78</v>
+      </c>
       <c r="F32" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G32" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="H32" s="62">
+      <c r="H32" s="61">
         <v>1.9120520000000001E-7</v>
       </c>
       <c r="I32" s="59"/>
-      <c r="K32" s="60"/>
-    </row>
-    <row r="33" spans="1:11">
+    </row>
+    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B33"/>
+      <c r="B33" t="s">
+        <v>71</v>
+      </c>
       <c r="C33" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D33" s="51">
         <v>3</v>
       </c>
-      <c r="E33"/>
+      <c r="E33" t="s">
+        <v>78</v>
+      </c>
       <c r="F33" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G33" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="H33" s="64">
+      <c r="H33" s="63">
         <v>-70.945670000000007</v>
       </c>
       <c r="I33" s="59"/>
-      <c r="K33" s="60"/>
-    </row>
-    <row r="34" spans="1:11">
+    </row>
+    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B34"/>
+      <c r="B34" t="s">
+        <v>71</v>
+      </c>
       <c r="C34" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D34" s="51">
         <v>3</v>
       </c>
-      <c r="E34"/>
+      <c r="E34" t="s">
+        <v>78</v>
+      </c>
       <c r="F34" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G34" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H34" s="64">
+      <c r="H34" s="63">
         <v>5.0880740000000001E-2</v>
       </c>
       <c r="I34" s="59"/>
-      <c r="K34" s="60"/>
-    </row>
-    <row r="35" spans="1:11">
+    </row>
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B35"/>
+      <c r="B35" t="s">
+        <v>71</v>
+      </c>
       <c r="C35" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D35" s="51">
         <v>3</v>
       </c>
-      <c r="E35"/>
+      <c r="E35" t="s">
+        <v>78</v>
+      </c>
       <c r="F35" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G35" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="H35" s="64">
+      <c r="H35" s="63">
         <v>-4.635052E-7</v>
       </c>
       <c r="I35" s="59"/>
-      <c r="K35" s="60"/>
-    </row>
-    <row r="36" spans="1:11">
+    </row>
+    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B36"/>
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
       <c r="C36" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D36" s="51">
         <v>3</v>
       </c>
-      <c r="E36"/>
+      <c r="E36" t="s">
+        <v>78</v>
+      </c>
       <c r="F36" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G36" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="H36" s="64">
+      <c r="H36" s="63">
         <v>525200.69999999995</v>
       </c>
       <c r="I36" s="59"/>
-      <c r="K36" s="60"/>
-    </row>
-    <row r="37" spans="1:11">
+    </row>
+    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B37"/>
+      <c r="B37" t="s">
+        <v>71</v>
+      </c>
       <c r="C37" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D37" s="51">
         <v>3</v>
       </c>
-      <c r="E37"/>
+      <c r="E37" t="s">
+        <v>78</v>
+      </c>
       <c r="F37" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G37" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="H37" s="64">
+      <c r="H37" s="63">
         <v>10.56958</v>
       </c>
       <c r="I37" s="59"/>
-      <c r="K37" s="60"/>
-    </row>
-    <row r="38" spans="1:11">
+    </row>
+    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B38"/>
+      <c r="B38" t="s">
+        <v>71</v>
+      </c>
       <c r="C38" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D38" s="51">
         <v>3</v>
       </c>
-      <c r="E38"/>
+      <c r="E38" t="s">
+        <v>78</v>
+      </c>
       <c r="F38" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G38" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="H38" s="64">
+      <c r="H38" s="63">
         <v>-0.120202</v>
       </c>
       <c r="I38" s="59"/>
-      <c r="K38" s="60"/>
-    </row>
-    <row r="39" spans="1:11">
+    </row>
+    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B39"/>
+      <c r="B39" t="s">
+        <v>71</v>
+      </c>
       <c r="C39" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D39" s="51">
         <v>3</v>
       </c>
-      <c r="E39"/>
+      <c r="E39" t="s">
+        <v>78</v>
+      </c>
       <c r="F39" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G39" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="H39" s="64">
+      <c r="H39" s="63">
         <v>25.338249999999999</v>
       </c>
       <c r="I39" s="59"/>
-      <c r="K39" s="60"/>
-    </row>
-    <row r="40" spans="1:11">
+    </row>
+    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B40"/>
+      <c r="B40" t="s">
+        <v>71</v>
+      </c>
       <c r="C40" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D40" s="51">
         <v>3</v>
       </c>
-      <c r="E40"/>
+      <c r="E40" t="s">
+        <v>78</v>
+      </c>
       <c r="F40" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G40" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H40" s="64">
+      <c r="H40" s="63">
         <v>-1.5499999999999999E-3</v>
       </c>
       <c r="I40" s="59"/>
-      <c r="K40" s="60"/>
-    </row>
-    <row r="41" spans="1:11">
+    </row>
+    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B41"/>
+      <c r="B41" t="s">
+        <v>71</v>
+      </c>
       <c r="C41" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D41" s="51">
         <v>3</v>
       </c>
-      <c r="E41"/>
+      <c r="E41" t="s">
+        <v>78</v>
+      </c>
       <c r="F41" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G41" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="H41" s="64">
+      <c r="H41" s="63">
         <v>0</v>
       </c>
       <c r="I41" s="59"/>
-      <c r="K41" s="60"/>
-    </row>
-    <row r="42" spans="1:11">
+    </row>
+    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B42"/>
+      <c r="B42" t="s">
+        <v>71</v>
+      </c>
       <c r="C42" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D42" s="51">
         <v>3</v>
       </c>
-      <c r="E42"/>
+      <c r="E42" t="s">
+        <v>78</v>
+      </c>
       <c r="F42" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G42" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="H42" s="64">
+      <c r="H42" s="63">
         <v>0.85476750000000001</v>
       </c>
       <c r="I42" s="59"/>
-      <c r="K42" s="60"/>
-    </row>
-    <row r="43" spans="1:11">
+    </row>
+    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B43"/>
+      <c r="B43" t="s">
+        <v>71</v>
+      </c>
       <c r="C43" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D43" s="51">
         <v>3</v>
       </c>
-      <c r="E43"/>
+      <c r="E43" t="s">
+        <v>78</v>
+      </c>
       <c r="F43" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G43" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H43" s="64">
+      <c r="H43" s="63">
         <v>4.4749189999999999E-3</v>
       </c>
       <c r="I43" s="59"/>
-      <c r="K43" s="60"/>
-    </row>
-    <row r="44" spans="1:11">
+    </row>
+    <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B44"/>
+      <c r="B44" t="s">
+        <v>71</v>
+      </c>
       <c r="C44" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D44" s="51">
         <v>3</v>
       </c>
-      <c r="E44"/>
+      <c r="E44" t="s">
+        <v>78</v>
+      </c>
       <c r="F44" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G44" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="H44" s="64">
+      <c r="H44" s="63">
         <v>-1.4537940000000001E-11</v>
       </c>
       <c r="I44" s="59"/>
-      <c r="K44" s="60"/>
-    </row>
-    <row r="45" spans="1:11">
+    </row>
+    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B45"/>
+      <c r="B45" t="s">
+        <v>71</v>
+      </c>
       <c r="C45" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D45" s="51">
         <v>3</v>
       </c>
-      <c r="E45"/>
+      <c r="E45" t="s">
+        <v>78</v>
+      </c>
       <c r="F45" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G45" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="64">
+      <c r="H45" s="63">
         <v>-0.99894559999999999</v>
       </c>
       <c r="I45" s="59"/>
-      <c r="K45" s="60"/>
-    </row>
-    <row r="46" spans="1:11">
+    </row>
+    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B46"/>
+      <c r="B46" t="s">
+        <v>71</v>
+      </c>
       <c r="C46" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D46" s="51">
         <v>3</v>
       </c>
-      <c r="E46"/>
+      <c r="E46" t="s">
+        <v>78</v>
+      </c>
       <c r="F46" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G46" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="H46" s="64">
+      <c r="H46" s="63">
         <v>0.16630900000000001</v>
       </c>
       <c r="I46" s="59"/>
-      <c r="K46" s="60"/>
-    </row>
-    <row r="47" spans="1:11">
+    </row>
+    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B47"/>
+      <c r="B47" t="s">
+        <v>71</v>
+      </c>
       <c r="C47" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D47" s="51">
         <v>3</v>
       </c>
-      <c r="E47"/>
+      <c r="E47" t="s">
+        <v>78</v>
+      </c>
       <c r="F47" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G47" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="H47" s="64">
+      <c r="H47" s="63">
         <v>-5.1783289999999995E-4</v>
       </c>
       <c r="I47" s="59"/>
-      <c r="K47" s="60"/>
-    </row>
-    <row r="48" spans="1:11">
+    </row>
+    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B48"/>
+      <c r="B48" t="s">
+        <v>71</v>
+      </c>
       <c r="C48" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D48" s="51">
         <v>3</v>
       </c>
-      <c r="E48"/>
+      <c r="E48" t="s">
+        <v>78</v>
+      </c>
       <c r="F48" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G48" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="H48" s="64">
+      <c r="H48" s="63">
         <v>6.6457530000000001E-5</v>
       </c>
       <c r="I48" s="59"/>
-      <c r="K48" s="60"/>
-    </row>
-    <row r="49" spans="1:11">
+    </row>
+    <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B49"/>
+      <c r="B49" t="s">
+        <v>71</v>
+      </c>
       <c r="C49" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D49" s="51">
         <v>3</v>
       </c>
-      <c r="E49"/>
+      <c r="E49" t="s">
+        <v>78</v>
+      </c>
       <c r="F49" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G49" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="H49" s="64">
+      <c r="H49" s="63">
         <v>-9.5700000000000003E-8</v>
       </c>
       <c r="I49" s="59"/>
-      <c r="K49" s="60"/>
-    </row>
-    <row r="50" spans="1:11">
+    </row>
+    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B50"/>
+      <c r="B50" t="s">
+        <v>71</v>
+      </c>
       <c r="C50" s="49" t="s">
         <v>44</v>
       </c>
       <c r="D50" s="51">
         <v>3</v>
       </c>
-      <c r="E50"/>
+      <c r="E50" t="s">
+        <v>78</v>
+      </c>
       <c r="F50" s="54" t="s">
         <v>47</v>
       </c>
       <c r="G50" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="H50" s="64">
+      <c r="H50" s="63">
         <v>3.2499999999999998E-6</v>
       </c>
       <c r="I50" s="59"/>
-      <c r="K50" s="60"/>
-    </row>
-    <row r="51" spans="1:11">
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="32"/>
       <c r="B51" s="32"/>
       <c r="C51" s="49"/>
@@ -2752,26 +2934,30 @@
       <c r="E51" s="4"/>
       <c r="F51" s="29"/>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B52"/>
+      <c r="B52" t="s">
+        <v>71</v>
+      </c>
       <c r="C52" s="48" t="s">
         <v>44</v>
       </c>
       <c r="D52" s="17">
         <v>3</v>
       </c>
-      <c r="E52" s="3"/>
-      <c r="F52" s="66">
+      <c r="E52" t="s">
+        <v>80</v>
+      </c>
+      <c r="F52" s="65">
         <v>13283</v>
       </c>
       <c r="G52" s="45"/>
       <c r="H52" s="45"/>
       <c r="I52" s="34"/>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="33"/>
       <c r="B53" s="33"/>
       <c r="C53" s="48"/>
@@ -2782,18 +2968,22 @@
       <c r="H53" s="45"/>
       <c r="I53" s="34"/>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B54"/>
+      <c r="B54" t="s">
+        <v>71</v>
+      </c>
       <c r="C54" s="48" t="s">
         <v>44</v>
       </c>
       <c r="D54" s="17">
         <v>3</v>
       </c>
-      <c r="E54"/>
+      <c r="E54" t="s">
+        <v>79</v>
+      </c>
       <c r="F54" s="52" t="s">
         <v>46</v>
       </c>
@@ -2803,10 +2993,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I55" s="3"/>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H60" s="12"/>
     </row>
   </sheetData>

</xml_diff>